<commit_message>
Added DateCreator to CommonHeadWithDynamicDataParserDataBaseUpdater
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Ex.xlsx
+++ b/src/main/resources/excel/Ex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Java\ExcelParser\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Java\ExcelParser\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -55,9 +55,6 @@
   <si>
     <t>company2</t>
   </si>
-  <si>
-    <t>date</t>
-  </si>
 </sst>
 </file>
 
@@ -81,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,61 +101,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -441,802 +391,735 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G4" s="1">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J4" s="1">
-        <v>15</v>
-      </c>
-      <c r="K4" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="1">
+        <v>11</v>
+      </c>
       <c r="D5" s="1">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G5" s="1">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1">
-        <v>20</v>
-      </c>
-      <c r="K5" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
-        <v>44599</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
       <c r="D6" s="1">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I6" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" s="1">
-        <v>25</v>
-      </c>
-      <c r="K6" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="1">
+        <v>13</v>
+      </c>
       <c r="D7" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="H7" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I7" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1">
-        <v>30</v>
-      </c>
-      <c r="K7" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C8" s="1">
+        <v>14</v>
+      </c>
       <c r="D8" s="1">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H8" s="1">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J8" s="1">
-        <v>35</v>
-      </c>
-      <c r="K8" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
-        <v>44599</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C9" s="1">
+        <v>15</v>
+      </c>
       <c r="D9" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="H9" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="J9" s="1">
-        <v>40</v>
-      </c>
-      <c r="K9" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C10" s="1">
+        <v>16</v>
+      </c>
       <c r="D10" s="1">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G10" s="1">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="H10" s="1">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="J10" s="1">
-        <v>45</v>
-      </c>
-      <c r="K10" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C11" s="1">
+        <v>17</v>
+      </c>
       <c r="D11" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G11" s="1">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="H11" s="1">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I11" s="1">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="J11" s="1">
-        <v>50</v>
-      </c>
-      <c r="K11" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
-        <v>44599</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C12" s="1">
+        <v>18</v>
+      </c>
       <c r="D12" s="1">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I12" s="1">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="J12" s="1">
-        <v>55</v>
-      </c>
-      <c r="K12" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C13" s="1">
+        <v>19</v>
+      </c>
       <c r="D13" s="1">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="H13" s="1">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I13" s="1">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="J13" s="1">
-        <v>60</v>
-      </c>
-      <c r="K13" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C14" s="1">
+        <v>20</v>
+      </c>
       <c r="D14" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G14" s="1">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="H14" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="I14" s="1">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="J14" s="1">
-        <v>65</v>
-      </c>
-      <c r="K14" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
-        <v>44599</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C15" s="1">
+        <v>21</v>
+      </c>
       <c r="D15" s="1">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F15" s="1">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="J15" s="1">
-        <v>70</v>
-      </c>
-      <c r="K15" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C16" s="1">
+        <v>22</v>
+      </c>
       <c r="D16" s="1">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G16" s="1">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="H16" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I16" s="1">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="J16" s="1">
-        <v>75</v>
-      </c>
-      <c r="K16" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C17" s="1">
+        <v>23</v>
+      </c>
       <c r="D17" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F17" s="1">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="H17" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I17" s="1">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="J17" s="1">
-        <v>80</v>
-      </c>
-      <c r="K17" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
-        <v>44599</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C18" s="1">
+        <v>24</v>
+      </c>
       <c r="D18" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E18" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F18" s="1">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G18" s="1">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="I18" s="1">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="J18" s="1">
-        <v>85</v>
-      </c>
-      <c r="K18" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C19" s="1">
+        <v>25</v>
+      </c>
       <c r="D19" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F19" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G19" s="1">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="H19" s="1">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I19" s="1">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="J19" s="1">
-        <v>90</v>
-      </c>
-      <c r="K19" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C20" s="1">
+        <v>26</v>
+      </c>
       <c r="D20" s="1">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G20" s="1">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H20" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I20" s="1">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="J20" s="1">
-        <v>95</v>
-      </c>
-      <c r="K20" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B21" s="2">
-        <v>44599</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C21" s="1">
+        <v>27</v>
+      </c>
       <c r="D21" s="1">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F21" s="1">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G21" s="1">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="H21" s="1">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I21" s="1">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="J21" s="1">
-        <v>100</v>
-      </c>
-      <c r="K21" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B22" s="2">
-        <v>44597</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C22" s="1">
+        <v>28</v>
+      </c>
       <c r="D22" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E22" s="1">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F22" s="1">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G22" s="1">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="H22" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I22" s="1">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="J22" s="1">
-        <v>105</v>
-      </c>
-      <c r="K22" s="1">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" s="2">
-        <v>44598</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C23" s="1">
+        <v>29</v>
+      </c>
       <c r="D23" s="1">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E23" s="1">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F23" s="1">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="G23" s="1">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="H23" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="I23" s="1">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="J23" s="1">
-        <v>110</v>
-      </c>
-      <c r="K23" s="1">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C1:C3"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>